<commit_message>
Reworked wire script to be compatible with battery sizing.
</commit_message>
<xml_diff>
--- a/wire_sizing_parameters.xlsx
+++ b/wire_sizing_parameters.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\OneDrive\Documents\GitHub\PSPL_R4_Avionics_Sizing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0DCCF23-6D35-48A3-8AC4-CDB6F27F9D2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97A6E6C-0F0E-45F9-BA78-608BEABE79F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{0C929514-014E-407F-B707-EB311BEEE485}"/>
+    <workbookView xWindow="4968" yWindow="1752" windowWidth="17280" windowHeight="8964" xr2:uid="{0C929514-014E-407F-B707-EB311BEEE485}"/>
   </bookViews>
   <sheets>
     <sheet name="Script Inputs" sheetId="1" r:id="rId1"/>
     <sheet name="Material Properties" sheetId="3" r:id="rId2"/>
     <sheet name="Wire Options" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="104">
   <si>
     <t>Density</t>
   </si>
@@ -115,39 +115,18 @@
     <t>Polytetrafluoroethylene (PTFE)</t>
   </si>
   <si>
-    <t>Solid</t>
-  </si>
-  <si>
     <t>100 ft</t>
   </si>
   <si>
-    <t>Blue</t>
-  </si>
-  <si>
     <t>Hook-up Wire</t>
   </si>
   <si>
-    <t>https://www.mouser.com/ProductDetail/Alpha-Wire/2855-1-BL005?qs=iXL3lsaaSSD7NPTu%2F3iINA%3D%3D&amp;utm_source=mouser-refine-download&amp;utm_medium=file&amp;utm_campaign=2855%2F1%20BL005&amp;utm_content=Alpha-Wire</t>
-  </si>
-  <si>
     <t>RoHS Compliant</t>
   </si>
   <si>
-    <t>14  In Stock</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/datasheet/2/14/1_Tech_Data-3533231.pdf</t>
-  </si>
-  <si>
     <t>Alpha Wire</t>
   </si>
   <si>
-    <t>2855/1 BL005</t>
-  </si>
-  <si>
-    <t>602-2855/1-100-06</t>
-  </si>
-  <si>
     <t>602-3116133-100</t>
   </si>
   <si>
@@ -347,6 +326,30 @@
   </si>
   <si>
     <t>HU WIRE TEFLON</t>
+  </si>
+  <si>
+    <t>AWG</t>
+  </si>
+  <si>
+    <t>Conductor Diameter (inch)</t>
+  </si>
+  <si>
+    <t>602-3114133-100</t>
+  </si>
+  <si>
+    <t>3114133 TN005</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/datasheet/2/14/Alpha_Wire_3114133_Tech_Data-3533209.pdf</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Alpha-Wire/3114133-TN005?qs=T6B9nY5N7E5GV%252Bf%2Flm5XXw%3D%3D&amp;utm_source=mouser-refine-download&amp;utm_medium=file&amp;utm_campaign=3114133%20TN005&amp;utm_content=Alpha-Wire</t>
+  </si>
+  <si>
+    <t>133 x 25</t>
+  </si>
+  <si>
+    <t>Estimated price</t>
   </si>
 </sst>
 </file>
@@ -384,7 +387,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -409,8 +412,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -526,12 +535,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -564,6 +599,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -573,10 +630,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -914,10 +974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F895DB8-3A4E-4FCF-8D34-90035BD53844}">
-  <dimension ref="B2:F14"/>
+  <dimension ref="B2:G14"/>
   <sheetViews>
-    <sheetView zoomScale="87" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="E1" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -926,7 +986,7 @@
     <col min="3" max="3" width="30.44140625" customWidth="1"/>
     <col min="4" max="4" width="42.109375" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" customWidth="1"/>
     <col min="7" max="7" width="45" customWidth="1"/>
     <col min="8" max="8" width="21.88671875" customWidth="1"/>
     <col min="9" max="9" width="16.44140625" customWidth="1"/>
@@ -936,28 +996,36 @@
     <col min="13" max="13" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" ht="16.8" x14ac:dyDescent="0.3">
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="14" t="s">
+    <row r="3" spans="2:7" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="14"/>
+      <c r="C3" s="22"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="12" t="s">
+    <row r="4" spans="2:7" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="13"/>
+      <c r="C4" s="21"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="E4" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
@@ -965,9 +1033,17 @@
         <v>2200</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="E5" s="3">
+        <v>10</v>
+      </c>
+      <c r="F5" s="17">
+        <v>2.9972000000000002E-3</v>
+      </c>
+      <c r="G5" s="25">
+        <v>1262.68</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
@@ -975,9 +1051,17 @@
         <v>0.30399999999999999</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="E6" s="5">
+        <v>8</v>
+      </c>
+      <c r="F6" s="18">
+        <v>4.3179999999999998E-3</v>
+      </c>
+      <c r="G6" s="24">
+        <v>3646.34</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -985,9 +1069,17 @@
         <v>1500</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E7" s="5">
+        <v>6</v>
+      </c>
+      <c r="F7" s="18">
+        <v>5.3340000000000002E-3</v>
+      </c>
+      <c r="G7" s="24">
+        <v>3818.49</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
         <v>8</v>
       </c>
@@ -995,17 +1087,25 @@
         <v>7.6199999999999998E-4</v>
       </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="12" t="s">
+      <c r="E8" s="7">
+        <v>4</v>
+      </c>
+      <c r="F8" s="19">
+        <v>6.8072000000000002E-3</v>
+      </c>
+      <c r="G8" s="23">
+        <v>6437.12</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="13"/>
+      <c r="C9" s="21"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
@@ -1015,7 +1115,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>7</v>
       </c>
@@ -1025,7 +1125,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
@@ -1035,7 +1135,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
         <v>12</v>
       </c>
@@ -1044,7 +1144,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:7" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="9" t="s">
         <v>13</v>
       </c>
@@ -1059,6 +1159,7 @@
     <mergeCell ref="B3:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1067,7 +1168,7 @@
   <dimension ref="B2:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1139,7 +1240,7 @@
       <c r="C17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="13" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1168,7 +1269,7 @@
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="12" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1204,8 +1305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1B9003F-AE97-41FB-8914-E9864EB590C2}">
   <dimension ref="B2:U15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+    <sheetView topLeftCell="E3" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1214,105 +1315,106 @@
     <col min="2" max="2" width="42.6640625" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="76.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" t="s">
         <v>50</v>
       </c>
-      <c r="C2" t="s">
+      <c r="J2" t="s">
         <v>51</v>
       </c>
-      <c r="D2" t="s">
+      <c r="K2" t="s">
         <v>52</v>
       </c>
-      <c r="E2" t="s">
+      <c r="L2" t="s">
         <v>53</v>
       </c>
-      <c r="F2" t="s">
+      <c r="M2" t="s">
         <v>54</v>
       </c>
-      <c r="G2" t="s">
+      <c r="N2" t="s">
         <v>55</v>
       </c>
-      <c r="H2" t="s">
+      <c r="O2" t="s">
         <v>56</v>
-      </c>
-      <c r="I2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J2" t="s">
-        <v>58</v>
-      </c>
-      <c r="K2" t="s">
-        <v>59</v>
-      </c>
-      <c r="L2" t="s">
-        <v>60</v>
-      </c>
-      <c r="M2" t="s">
-        <v>61</v>
-      </c>
-      <c r="N2" t="s">
-        <v>62</v>
-      </c>
-      <c r="O2" t="s">
-        <v>63</v>
       </c>
       <c r="P2" t="s">
         <v>5</v>
       </c>
       <c r="Q2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="R2" t="s">
         <v>16</v>
       </c>
       <c r="S2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>35</v>
+        <v>98</v>
       </c>
       <c r="C4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" t="str">
+        <f>"$6,437.12"</f>
+        <v>$6,437.12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" t="s">
+        <v>101</v>
+      </c>
+      <c r="K4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" ref="L4" si="0">"4 AWG"</f>
+        <v>4 AWG</v>
+      </c>
+      <c r="M4" t="s">
         <v>34</v>
       </c>
-      <c r="D4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" t="str">
-        <f>"$194.48"</f>
-        <v>$194.48</v>
-      </c>
-      <c r="H4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" t="str">
-        <f>"22 AWG"</f>
-        <v>22 AWG</v>
-      </c>
-      <c r="M4" t="s">
-        <v>27</v>
-      </c>
       <c r="N4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O4" t="s">
-        <v>25</v>
+        <v>102</v>
       </c>
       <c r="P4" t="s">
         <v>24</v>
@@ -1321,60 +1423,56 @@
         <v>23</v>
       </c>
       <c r="R4" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="S4" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="T4" t="s">
-        <v>20</v>
-      </c>
-      <c r="U4" t="str">
-        <f>"2855"</f>
-        <v>2855</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" t="s">
-        <v>38</v>
+        <v>28</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>31</v>
       </c>
       <c r="F6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G6" t="str">
         <f>"$3,818.49"</f>
         <v>$3,818.49</v>
       </c>
       <c r="H6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="K6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L6" t="str">
         <f>"6 AWG"</f>
         <v>6 AWG</v>
       </c>
       <c r="M6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="N6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O6" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="P6" t="s">
         <v>24</v>
@@ -1383,53 +1481,53 @@
         <v>23</v>
       </c>
       <c r="R6" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="S6" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" t="s">
-        <v>47</v>
+        <v>28</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="F7" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G7" t="str">
         <f>"$2,207.51"</f>
         <v>$2,207.51</v>
       </c>
       <c r="H7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J7" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="K7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L7" t="str">
         <f>"6 AWG"</f>
         <v>6 AWG</v>
       </c>
       <c r="M7" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="N7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O7" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="P7" t="s">
         <v>24</v>
@@ -1438,53 +1536,53 @@
         <v>23</v>
       </c>
       <c r="R7" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="S7" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" t="s">
-        <v>68</v>
+        <v>28</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>61</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G9" t="str">
         <f>"$3,646.34"</f>
         <v>$3,646.34</v>
       </c>
       <c r="H9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J9" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="K9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L9" t="str">
         <f>"8 AWG"</f>
         <v>8 AWG</v>
       </c>
       <c r="M9" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="N9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O9" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="P9" t="s">
         <v>24</v>
@@ -1493,53 +1591,53 @@
         <v>23</v>
       </c>
       <c r="S9" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="T9" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" t="s">
-        <v>73</v>
+        <v>28</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>66</v>
       </c>
       <c r="F10" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G10" t="str">
         <f>"$1,664.42"</f>
         <v>$1,664.42</v>
       </c>
       <c r="H10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J10" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="K10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L10" t="str">
         <f>"8 AWG"</f>
         <v>8 AWG</v>
       </c>
       <c r="M10" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="N10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O10" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="P10" t="s">
         <v>24</v>
@@ -1548,10 +1646,10 @@
         <v>23</v>
       </c>
       <c r="R10" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="T10" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="U10" t="str">
         <f>"3138"</f>
@@ -1560,45 +1658,45 @@
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" t="s">
-        <v>78</v>
+        <v>28</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>71</v>
       </c>
       <c r="F12" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G12" t="str">
         <f>"$1,262.68"</f>
         <v>$1,262.68</v>
       </c>
       <c r="H12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J12" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="K12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L12" t="str">
         <f>"10 AWG"</f>
         <v>10 AWG</v>
       </c>
       <c r="M12" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="N12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O12" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="P12" t="s">
         <v>24</v>
@@ -1622,45 +1720,45 @@
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C13" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" t="s">
-        <v>85</v>
+        <v>28</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>78</v>
       </c>
       <c r="F13" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G13" t="str">
         <f>"$1,092.84"</f>
         <v>$1,092.84</v>
       </c>
       <c r="H13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J13" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="K13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L13" t="str">
         <f>"10 AWG"</f>
         <v>10 AWG</v>
       </c>
       <c r="M13" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="N13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O13" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="P13" t="s">
         <v>24</v>
@@ -1669,10 +1767,10 @@
         <v>23</v>
       </c>
       <c r="R13" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="T13" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="U13" t="str">
         <f>"3131"</f>
@@ -1681,45 +1779,45 @@
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C14" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" t="s">
-        <v>91</v>
+        <v>28</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>84</v>
       </c>
       <c r="F14" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G14" t="str">
         <f>"$1,594.27"</f>
         <v>$1,594.27</v>
       </c>
       <c r="H14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J14" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="K14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L14" t="str">
         <f>"10 AWG"</f>
         <v>10 AWG</v>
       </c>
       <c r="M14" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="N14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O14" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="P14" t="s">
         <v>24</v>
@@ -1728,10 +1826,10 @@
         <v>23</v>
       </c>
       <c r="S14" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="T14" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="U14" t="str">
         <f>"3111"</f>
@@ -1740,48 +1838,48 @@
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C15" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" t="s">
-        <v>96</v>
+        <v>28</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>89</v>
       </c>
       <c r="F15" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G15" t="str">
         <f>"$1,680.97"</f>
         <v>$1,680.97</v>
       </c>
       <c r="H15" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I15" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="J15" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="K15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L15" t="str">
         <f>"10 AWG"</f>
         <v>10 AWG</v>
       </c>
       <c r="M15" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="N15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O15" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="P15" t="s">
         <v>24</v>
@@ -1799,10 +1897,21 @@
         <v>20</v>
       </c>
       <c r="U15" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E6" r:id="rId1" xr:uid="{66BF92C1-91B7-4E7E-9ED9-2879C212DB4A}"/>
+    <hyperlink ref="E15" r:id="rId2" xr:uid="{D2A1FC41-93B0-48D3-A926-0AC3B4B49B45}"/>
+    <hyperlink ref="E14" r:id="rId3" xr:uid="{29AC16EB-7703-4D4E-BE32-792ACA2DFDA1}"/>
+    <hyperlink ref="E13" r:id="rId4" xr:uid="{ADA4393A-7CC4-4879-8725-E82351BD83B1}"/>
+    <hyperlink ref="E12" r:id="rId5" xr:uid="{0AFBC84E-9292-4E03-B7C4-E97E0CBBBFE7}"/>
+    <hyperlink ref="E10" r:id="rId6" xr:uid="{787019BD-2A54-4BE9-86B4-3203EA30D51C}"/>
+    <hyperlink ref="E9" r:id="rId7" xr:uid="{9F52F2BF-7181-4318-ADE8-38D2AEAEF3AE}"/>
+    <hyperlink ref="E7" r:id="rId8" xr:uid="{5C2F9BB5-450E-4E04-81C3-DA4259353A1E}"/>
+    <hyperlink ref="E4" r:id="rId9" xr:uid="{A4E12C9D-492F-4AF0-99BE-DB1151172EB9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>